<commit_message>
add for simple char device driver module
</commit_message>
<xml_diff>
--- a/Linux/DeviceDrivers/iAuto/0.如何编写一个简单的模块.xlsx
+++ b/Linux/DeviceDrivers/iAuto/0.如何编写一个简单的模块.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,17 @@
     <sheet name="hello.c" sheetId="8" r:id="rId3"/>
     <sheet name="drivers_ylm_hello_Kconfig" sheetId="7" r:id="rId4"/>
     <sheet name="drivers_ylm_Kconfig" sheetId="6" r:id="rId5"/>
-    <sheet name="drivers_Kconfig" sheetId="5" r:id="rId6"/>
-    <sheet name="Makefile" sheetId="9" r:id="rId7"/>
-    <sheet name="xxx_defconfig" sheetId="3" r:id="rId8"/>
+    <sheet name="drivers_ylm_Makefile" sheetId="9" r:id="rId6"/>
+    <sheet name="drivers_Kconfig" sheetId="5" r:id="rId7"/>
+    <sheet name="drivers_Makefile" sheetId="10" r:id="rId8"/>
+    <sheet name="xxx_defconfig" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>1. 需要修改或添加的文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,22 +144,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4. drivers/Kconfig</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. drivers/Makefile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>./buld/target/build-kernel-xxx.sh menuconfig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>=&gt; 6. arch/arm/configs/xxx_defconfig</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>config YLM_HELLO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,10 +200,31 @@
     <t>module_exit(hello_exit);</t>
   </si>
   <si>
+    <t xml:space="preserve">余注: config 就是一个选项, 在 menuconfig 中可见, 层级依赖 Kconfig 中 source </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. drivers/ylm/Makefile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. drivers/Kconfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. drivers/Makefile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=&gt; 7. arch/arm/configs/xxx_defconfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>obj-$(CONFIG_YLM_HELLO) += hello/hello.o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">余注: config 就是一个选项, 在 menuconfig 中可见, 层级依赖 Kconfig 中 source </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>obj-$(CONFIG_YLM_HELLO) += ylm/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -573,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE29" sqref="AE29"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="11.25"/>
@@ -651,22 +661,27 @@
     </row>
     <row r="16" spans="2:4">
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="3:3">
-      <c r="C19" s="2" t="s">
-        <v>33</v>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -741,7 +756,7 @@
     </row>
     <row r="15" spans="2:3">
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -766,72 +781,72 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -855,22 +870,22 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -918,6 +933,30 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="16384" width="2.625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
@@ -937,12 +976,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="11.25"/>
@@ -952,16 +991,17 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B5"/>
   <sheetViews>

</xml_diff>